<commit_message>
fixed HUD, OSHRC, PC, Treasury, USADF, USTR
</commit_message>
<xml_diff>
--- a/contacts/usagov-data/foiaHub-usaContacts-matches.xlsx
+++ b/contacts/usagov-data/foiaHub-usaContacts-matches.xlsx
@@ -1774,6 +1774,9 @@
     <t>http://www.usa.gov/directory/federal/african-development-foundation.shtml</t>
   </si>
   <si>
+    <t>USADF</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -1792,6 +1795,9 @@
     <t>http://www.usa.gov/directory/federal/occupational-safety-and-health-review-commission.shtml</t>
   </si>
   <si>
+    <t>OSHRC</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -2392,6 +2398,9 @@
     <t>http://www.usa.gov/directory/federal/peace-corps.shtml</t>
   </si>
   <si>
+    <t>PC</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -2794,6 +2803,9 @@
     <t>http://www.treasury.gov/</t>
   </si>
   <si>
+    <t>Treasury</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -2927,6 +2939,9 @@
   </si>
   <si>
     <t>http://www.ustr.gov/</t>
+  </si>
+  <si>
+    <t>USTR</t>
   </si>
   <si>
     <t>fh_name</t>
@@ -3092,7 +3107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -3120,6 +3135,11 @@
     </font>
     <font>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF1155CC"/>
     </font>
     <font>
       <u/>
@@ -3185,7 +3205,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -3213,6 +3233,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="9">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
@@ -6067,1107 +6090,1104 @@
       </c>
     </row>
     <row r="95">
-      <c t="s" s="1" r="A95">
+      <c t="s" s="3" r="A95">
         <v>568</v>
       </c>
-      <c s="1" r="B95">
+      <c s="3" r="B95">
         <v>144.0</v>
       </c>
-      <c t="s" s="1" r="C95">
+      <c t="s" s="3" r="C95">
         <v>569</v>
       </c>
-      <c t="s" s="2" r="D95">
+      <c t="s" s="4" r="D95">
         <v>570</v>
       </c>
-      <c t="s" s="1" r="E95">
+      <c t="s" s="3" r="E95">
         <v>571</v>
       </c>
-      <c t="s" s="2" r="F95">
+      <c t="s" s="4" r="F95">
         <v>572</v>
       </c>
-      <c s="1" r="G95">
+      <c s="3" r="G95">
         <v>52581.0</v>
       </c>
-      <c t="s" s="2" r="H95">
+      <c t="s" s="4" r="H95">
         <v>573</v>
       </c>
-      <c t="str" r="I95">
-        <f ref="I95:I96" t="shared" si="3">iferror(iferror(REGEXEXTRACT(C95,"\((\w+)\)"),REGEXEXTRACT(E95,"\((\w+)\)")),"")</f>
-        <v/>
+      <c t="s" s="3" r="I95">
+        <v>574</v>
       </c>
     </row>
     <row r="96">
-      <c t="s" s="1" r="A96">
-        <v>574</v>
-      </c>
-      <c s="1" r="B96">
+      <c t="s" s="3" r="A96">
+        <v>575</v>
+      </c>
+      <c s="3" r="B96">
         <v>116.0</v>
       </c>
-      <c t="s" s="1" r="C96">
-        <v>575</v>
-      </c>
-      <c t="s" s="2" r="D96">
+      <c t="s" s="3" r="C96">
         <v>576</v>
       </c>
-      <c t="s" s="1" r="E96">
+      <c t="s" s="4" r="D96">
         <v>577</v>
       </c>
-      <c t="s" s="2" r="F96">
+      <c t="s" s="3" r="E96">
         <v>578</v>
       </c>
-      <c s="1" r="G96">
+      <c t="s" s="4" r="F96">
+        <v>579</v>
+      </c>
+      <c s="3" r="G96">
         <v>49577.0</v>
       </c>
-      <c t="s" s="2" r="H96">
-        <v>579</v>
-      </c>
-      <c t="str" r="I96">
+      <c t="s" s="4" r="H96">
+        <v>580</v>
+      </c>
+      <c t="s" s="3" r="I96">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="97">
+      <c t="s" s="3" r="A97">
+        <v>582</v>
+      </c>
+      <c s="3" r="B97">
+        <v>3.0</v>
+      </c>
+      <c t="s" s="3" r="C97">
+        <v>583</v>
+      </c>
+      <c t="s" s="4" r="D97">
+        <v>584</v>
+      </c>
+      <c t="s" s="3" r="E97">
+        <v>585</v>
+      </c>
+      <c t="s" s="4" r="F97">
+        <v>586</v>
+      </c>
+      <c s="3" r="G97">
+        <v>49093.0</v>
+      </c>
+      <c t="s" s="4" r="H97">
+        <v>587</v>
+      </c>
+      <c t="s" s="3" r="I97">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="98">
+      <c t="s" s="1" r="A98">
+        <v>589</v>
+      </c>
+      <c s="1" r="B98">
+        <v>78.0</v>
+      </c>
+      <c t="s" s="1" r="C98">
+        <v>590</v>
+      </c>
+      <c t="s" s="2" r="D98">
+        <v>591</v>
+      </c>
+      <c t="s" s="1" r="E98">
+        <v>592</v>
+      </c>
+      <c t="s" s="2" r="F98">
+        <v>593</v>
+      </c>
+      <c s="1" r="G98">
+        <v>49048.0</v>
+      </c>
+      <c t="s" s="2" r="H98">
+        <v>594</v>
+      </c>
+      <c t="str" r="I98">
+        <f ref="I98:I115" t="shared" si="3">iferror(iferror(REGEXEXTRACT(C98,"\((\w+)\)"),REGEXEXTRACT(E98,"\((\w+)\)")),"")</f>
+        <v>GSA</v>
+      </c>
+    </row>
+    <row r="99">
+      <c t="s" s="1" r="A99">
+        <v>595</v>
+      </c>
+      <c s="1" r="B99">
+        <v>31.0</v>
+      </c>
+      <c t="s" s="1" r="C99">
+        <v>596</v>
+      </c>
+      <c t="s" s="2" r="D99">
+        <v>597</v>
+      </c>
+      <c t="s" s="1" r="E99">
+        <v>598</v>
+      </c>
+      <c t="s" s="2" r="F99">
+        <v>599</v>
+      </c>
+      <c s="1" r="G99">
+        <v>48151.0</v>
+      </c>
+      <c t="s" s="2" r="H99">
+        <v>600</v>
+      </c>
+      <c t="str" r="I99">
+        <f t="shared" si="3"/>
+        <v>USPTO</v>
+      </c>
+    </row>
+    <row r="100">
+      <c t="s" s="1" r="A100">
+        <v>601</v>
+      </c>
+      <c s="1" r="B100">
+        <v>17.0</v>
+      </c>
+      <c t="s" s="1" r="C100">
+        <v>602</v>
+      </c>
+      <c t="s" s="2" r="D100">
+        <v>603</v>
+      </c>
+      <c t="s" s="1" r="E100">
+        <v>604</v>
+      </c>
+      <c t="s" s="2" r="F100">
+        <v>605</v>
+      </c>
+      <c s="1" r="G100">
+        <v>49149.0</v>
+      </c>
+      <c t="s" s="2" r="H100">
+        <v>606</v>
+      </c>
+      <c t="str" r="I100">
+        <f t="shared" si="3"/>
+        <v>USCG</v>
+      </c>
+    </row>
+    <row r="101">
+      <c t="s" s="1" r="A101">
+        <v>607</v>
+      </c>
+      <c s="1" r="B101">
+        <v>52.0</v>
+      </c>
+      <c t="s" s="1" r="C101">
+        <v>608</v>
+      </c>
+      <c t="s" s="2" r="D101">
+        <v>609</v>
+      </c>
+      <c t="s" s="1" r="E101">
+        <v>610</v>
+      </c>
+      <c t="s" s="2" r="F101">
+        <v>611</v>
+      </c>
+      <c s="1" r="G101">
+        <v>49126.0</v>
+      </c>
+      <c t="s" s="2" r="H101">
+        <v>612</v>
+      </c>
+      <c t="str" r="I101">
+        <f t="shared" si="3"/>
+        <v>BOP</v>
+      </c>
+    </row>
+    <row r="102">
+      <c t="s" s="1" r="A102">
+        <v>613</v>
+      </c>
+      <c s="1" r="B102">
+        <v>59.0</v>
+      </c>
+      <c t="s" s="1" r="C102">
+        <v>614</v>
+      </c>
+      <c t="s" s="1" r="D102">
+        <v>615</v>
+      </c>
+      <c t="s" s="1" r="E102">
+        <v>616</v>
+      </c>
+      <c t="s" s="2" r="F102">
+        <v>617</v>
+      </c>
+      <c s="1" r="G102">
+        <v>48032.0</v>
+      </c>
+      <c t="s" s="2" r="H102">
+        <v>618</v>
+      </c>
+      <c t="str" r="I102">
+        <f t="shared" si="3"/>
+        <v>EEOC</v>
+      </c>
+    </row>
+    <row r="103">
+      <c t="s" s="1" r="A103">
+        <v>619</v>
+      </c>
+      <c s="1" r="B103">
+        <v>81.0</v>
+      </c>
+      <c t="s" s="1" r="C103">
+        <v>620</v>
+      </c>
+      <c t="s" s="2" r="D103">
+        <v>621</v>
+      </c>
+      <c t="s" s="1" r="E103">
+        <v>622</v>
+      </c>
+      <c t="s" s="2" r="F103">
+        <v>623</v>
+      </c>
+      <c s="1" r="G103">
+        <v>49074.0</v>
+      </c>
+      <c t="s" s="2" r="H103">
+        <v>624</v>
+      </c>
+      <c t="str" r="I103">
+        <f t="shared" si="3"/>
+        <v>AHRQ</v>
+      </c>
+    </row>
+    <row r="104">
+      <c t="s" s="1" r="A104">
+        <v>625</v>
+      </c>
+      <c s="1" r="B104">
+        <v>111.0</v>
+      </c>
+      <c t="s" s="1" r="C104">
+        <v>626</v>
+      </c>
+      <c t="s" s="2" r="D104">
+        <v>627</v>
+      </c>
+      <c t="s" s="1" r="E104">
+        <v>628</v>
+      </c>
+      <c t="s" s="2" r="F104">
+        <v>629</v>
+      </c>
+      <c s="1" r="G104">
+        <v>49586.0</v>
+      </c>
+      <c t="s" s="2" r="H104">
+        <v>630</v>
+      </c>
+      <c t="str" r="I104">
+        <f t="shared" si="3"/>
+        <v>ONDCP</v>
+      </c>
+    </row>
+    <row r="105">
+      <c t="s" s="1" r="A105">
+        <v>631</v>
+      </c>
+      <c s="1" r="B105">
+        <v>6.0</v>
+      </c>
+      <c t="s" s="1" r="C105">
+        <v>632</v>
+      </c>
+      <c t="s" s="2" r="D105">
+        <v>633</v>
+      </c>
+      <c t="s" s="1" r="E105">
+        <v>634</v>
+      </c>
+      <c t="s" s="2" r="F105">
+        <v>635</v>
+      </c>
+      <c s="1" r="G105">
+        <v>49113.0</v>
+      </c>
+      <c t="s" s="2" r="H105">
+        <v>636</v>
+      </c>
+      <c t="str" r="I105">
+        <f t="shared" si="3"/>
+        <v>CFPB</v>
+      </c>
+    </row>
+    <row r="106">
+      <c t="s" s="1" r="A106">
+        <v>637</v>
+      </c>
+      <c s="1" r="B106">
+        <v>50.0</v>
+      </c>
+      <c t="s" s="1" r="C106">
+        <v>638</v>
+      </c>
+      <c t="s" s="2" r="D106">
+        <v>639</v>
+      </c>
+      <c t="s" s="1" r="E106">
+        <v>640</v>
+      </c>
+      <c t="s" s="2" r="F106">
+        <v>641</v>
+      </c>
+      <c s="1" r="G106">
+        <v>52688.0</v>
+      </c>
+      <c t="s" s="2" r="H106">
+        <v>642</v>
+      </c>
+      <c t="str" r="I106">
+        <f t="shared" si="3"/>
+        <v>DEA</v>
+      </c>
+    </row>
+    <row r="107">
+      <c t="s" s="1" r="A107">
+        <v>643</v>
+      </c>
+      <c s="1" r="B107">
+        <v>128.0</v>
+      </c>
+      <c t="s" s="1" r="C107">
+        <v>644</v>
+      </c>
+      <c t="s" s="2" r="D107">
+        <v>645</v>
+      </c>
+      <c t="s" s="1" r="E107">
+        <v>646</v>
+      </c>
+      <c t="s" s="2" r="F107">
+        <v>647</v>
+      </c>
+      <c s="1" r="G107">
+        <v>49691.0</v>
+      </c>
+      <c t="s" s="2" r="H107">
+        <v>648</v>
+      </c>
+      <c t="str" r="I107">
+        <f t="shared" si="3"/>
+        <v>STB</v>
+      </c>
+    </row>
+    <row r="108">
+      <c t="s" s="1" r="A108">
+        <v>649</v>
+      </c>
+      <c s="1" r="B108">
+        <v>98.0</v>
+      </c>
+      <c t="s" s="1" r="C108">
+        <v>650</v>
+      </c>
+      <c t="s" s="2" r="D108">
+        <v>651</v>
+      </c>
+      <c t="s" s="1" r="E108">
+        <v>652</v>
+      </c>
+      <c t="s" s="2" r="F108">
+        <v>653</v>
+      </c>
+      <c s="1" r="G108">
+        <v>52633.0</v>
+      </c>
+      <c t="s" s="2" r="H108">
+        <v>654</v>
+      </c>
+      <c t="str" r="I108">
+        <f t="shared" si="3"/>
+        <v>NCPC</v>
+      </c>
+    </row>
+    <row r="109">
+      <c t="s" s="1" r="A109">
+        <v>655</v>
+      </c>
+      <c s="1" r="B109">
+        <v>89.0</v>
+      </c>
+      <c t="s" s="1" r="C109">
+        <v>656</v>
+      </c>
+      <c t="s" s="1" r="D109">
+        <v>657</v>
+      </c>
+      <c t="s" s="1" r="E109">
+        <v>658</v>
+      </c>
+      <c t="s" s="2" r="F109">
+        <v>659</v>
+      </c>
+      <c s="1" r="G109">
+        <v>49618.0</v>
+      </c>
+      <c t="s" s="2" r="H109">
+        <v>660</v>
+      </c>
+      <c t="str" r="I109">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="97">
-      <c t="s" s="3" r="A97">
-        <v>580</v>
-      </c>
-      <c s="3" r="B97">
-        <v>3.0</v>
-      </c>
-      <c t="s" s="3" r="C97">
-        <v>581</v>
-      </c>
-      <c t="s" s="4" r="D97">
-        <v>582</v>
-      </c>
-      <c t="s" s="3" r="E97">
-        <v>583</v>
-      </c>
-      <c t="s" s="4" r="F97">
-        <v>584</v>
-      </c>
-      <c s="3" r="G97">
-        <v>49093.0</v>
-      </c>
-      <c t="s" s="4" r="H97">
-        <v>585</v>
-      </c>
-      <c t="s" s="3" r="I97">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="98">
-      <c t="s" s="1" r="A98">
-        <v>587</v>
-      </c>
-      <c s="1" r="B98">
-        <v>78.0</v>
-      </c>
-      <c t="s" s="1" r="C98">
-        <v>588</v>
-      </c>
-      <c t="s" s="2" r="D98">
-        <v>589</v>
-      </c>
-      <c t="s" s="1" r="E98">
-        <v>590</v>
-      </c>
-      <c t="s" s="2" r="F98">
-        <v>591</v>
-      </c>
-      <c s="1" r="G98">
-        <v>49048.0</v>
-      </c>
-      <c t="s" s="2" r="H98">
-        <v>592</v>
-      </c>
-      <c t="str" r="I98">
-        <f ref="I98:I115" t="shared" si="4">iferror(iferror(REGEXEXTRACT(C98,"\((\w+)\)"),REGEXEXTRACT(E98,"\((\w+)\)")),"")</f>
-        <v>GSA</v>
-      </c>
-    </row>
-    <row r="99">
-      <c t="s" s="1" r="A99">
-        <v>593</v>
-      </c>
-      <c s="1" r="B99">
-        <v>31.0</v>
-      </c>
-      <c t="s" s="1" r="C99">
-        <v>594</v>
-      </c>
-      <c t="s" s="2" r="D99">
-        <v>595</v>
-      </c>
-      <c t="s" s="1" r="E99">
-        <v>596</v>
-      </c>
-      <c t="s" s="2" r="F99">
-        <v>597</v>
-      </c>
-      <c s="1" r="G99">
-        <v>48151.0</v>
-      </c>
-      <c t="s" s="2" r="H99">
-        <v>598</v>
-      </c>
-      <c t="str" r="I99">
+    <row r="110">
+      <c t="s" s="1" r="A110">
+        <v>661</v>
+      </c>
+      <c s="1" r="B110">
+        <v>136.0</v>
+      </c>
+      <c t="s" s="1" r="C110">
+        <v>662</v>
+      </c>
+      <c t="s" s="2" r="D110">
+        <v>663</v>
+      </c>
+      <c t="s" s="1" r="E110">
+        <v>664</v>
+      </c>
+      <c t="s" s="2" r="F110">
+        <v>665</v>
+      </c>
+      <c s="1" r="G110">
+        <v>49013.0</v>
+      </c>
+      <c t="s" s="2" r="H110">
+        <v>666</v>
+      </c>
+      <c t="str" r="I110">
+        <f t="shared" si="3"/>
+        <v>CPSC</v>
+      </c>
+    </row>
+    <row r="111">
+      <c t="s" s="1" r="A111">
+        <v>667</v>
+      </c>
+      <c s="1" r="B111">
+        <v>94.0</v>
+      </c>
+      <c t="s" s="1" r="C111">
+        <v>668</v>
+      </c>
+      <c t="s" s="1" r="D111">
+        <v>669</v>
+      </c>
+      <c t="s" s="1" r="E111">
+        <v>670</v>
+      </c>
+      <c t="s" s="2" r="F111">
+        <v>671</v>
+      </c>
+      <c s="1" r="G111">
+        <v>52630.0</v>
+      </c>
+      <c t="s" s="2" r="H111">
+        <v>672</v>
+      </c>
+      <c t="str" r="I111">
+        <f t="shared" si="3"/>
+        <v>MSPB</v>
+      </c>
+    </row>
+    <row r="112">
+      <c t="s" s="1" r="A112">
+        <v>673</v>
+      </c>
+      <c s="1" r="B112">
+        <v>28.0</v>
+      </c>
+      <c t="s" s="1" r="C112">
+        <v>674</v>
+      </c>
+      <c t="s" s="2" r="D112">
+        <v>675</v>
+      </c>
+      <c t="s" s="1" r="E112">
+        <v>676</v>
+      </c>
+      <c t="s" s="2" r="F112">
+        <v>677</v>
+      </c>
+      <c s="1" r="G112">
+        <v>49517.0</v>
+      </c>
+      <c t="s" s="2" r="H112">
+        <v>678</v>
+      </c>
+      <c t="str" r="I112">
+        <f t="shared" si="3"/>
+        <v>NIST</v>
+      </c>
+    </row>
+    <row r="113">
+      <c t="s" s="1" r="A113">
+        <v>679</v>
+      </c>
+      <c s="1" r="B113">
+        <v>103.0</v>
+      </c>
+      <c t="s" s="1" r="C113">
+        <v>680</v>
+      </c>
+      <c t="s" s="2" r="D113">
+        <v>681</v>
+      </c>
+      <c t="s" s="1" r="E113">
+        <v>682</v>
+      </c>
+      <c t="s" s="2" r="F113">
+        <v>683</v>
+      </c>
+      <c s="1" r="G113">
+        <v>49523.0</v>
+      </c>
+      <c t="s" s="2" r="H113">
+        <v>684</v>
+      </c>
+      <c t="str" r="I113">
+        <f t="shared" si="3"/>
+        <v>NLRB</v>
+      </c>
+    </row>
+    <row r="114">
+      <c t="s" s="1" r="A114">
+        <v>685</v>
+      </c>
+      <c s="1" r="B114">
+        <v>63.0</v>
+      </c>
+      <c t="s" s="1" r="C114">
+        <v>686</v>
+      </c>
+      <c t="s" s="2" r="D114">
+        <v>687</v>
+      </c>
+      <c t="s" s="1" r="E114">
+        <v>688</v>
+      </c>
+      <c t="s" s="2" r="F114">
+        <v>689</v>
+      </c>
+      <c s="1" r="G114">
+        <v>49041.0</v>
+      </c>
+      <c t="s" s="2" r="H114">
+        <v>690</v>
+      </c>
+      <c t="str" r="I114">
+        <f t="shared" si="3"/>
+        <v>FCC</v>
+      </c>
+    </row>
+    <row r="115">
+      <c t="s" s="1" r="A115">
+        <v>691</v>
+      </c>
+      <c s="1" r="B115">
+        <v>95.0</v>
+      </c>
+      <c t="s" s="1" r="C115">
+        <v>692</v>
+      </c>
+      <c t="s" s="1" r="D115">
+        <v>693</v>
+      </c>
+      <c t="s" s="1" r="E115">
+        <v>694</v>
+      </c>
+      <c t="s" s="2" r="F115">
+        <v>695</v>
+      </c>
+      <c s="1" r="G115">
+        <v>49483.0</v>
+      </c>
+      <c t="s" s="2" r="H115">
+        <v>696</v>
+      </c>
+      <c t="str" r="I115">
+        <f t="shared" si="3"/>
+        <v>NARA</v>
+      </c>
+    </row>
+    <row r="116">
+      <c t="s" s="3" r="A116">
+        <v>697</v>
+      </c>
+      <c s="3" r="B116">
+        <v>75.0</v>
+      </c>
+      <c t="s" s="3" r="C116">
+        <v>698</v>
+      </c>
+      <c t="s" s="4" r="D116">
+        <v>699</v>
+      </c>
+      <c t="s" s="3" r="E116">
+        <v>700</v>
+      </c>
+      <c t="s" s="4" r="F116">
+        <v>701</v>
+      </c>
+      <c s="3" r="G116">
+        <v>49046.0</v>
+      </c>
+      <c t="s" s="4" r="H116">
+        <v>702</v>
+      </c>
+      <c t="s" s="3" r="I116">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="117">
+      <c t="s" s="1" r="A117">
+        <v>704</v>
+      </c>
+      <c s="1" r="B117">
+        <v>54.0</v>
+      </c>
+      <c t="s" s="1" r="C117">
+        <v>705</v>
+      </c>
+      <c t="s" s="2" r="D117">
+        <v>706</v>
+      </c>
+      <c t="s" s="1" r="E117">
+        <v>707</v>
+      </c>
+      <c t="s" s="2" r="F117">
+        <v>708</v>
+      </c>
+      <c s="1" r="G117">
+        <v>49451.0</v>
+      </c>
+      <c t="s" s="2" r="H117">
+        <v>709</v>
+      </c>
+      <c t="str" r="I117">
+        <f ref="I117:I128" t="shared" si="4">iferror(iferror(REGEXEXTRACT(C117,"\((\w+)\)"),REGEXEXTRACT(E117,"\((\w+)\)")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118">
+      <c t="s" s="1" r="A118">
+        <v>710</v>
+      </c>
+      <c s="1" r="B118">
+        <v>32.0</v>
+      </c>
+      <c t="s" s="1" r="C118">
+        <v>711</v>
+      </c>
+      <c t="s" s="1" r="D118">
+        <v>712</v>
+      </c>
+      <c t="s" s="1" r="E118">
+        <v>713</v>
+      </c>
+      <c t="s" s="2" r="F118">
+        <v>714</v>
+      </c>
+      <c s="1" r="G118">
+        <v>49229.0</v>
+      </c>
+      <c t="s" s="2" r="H118">
+        <v>715</v>
+      </c>
+      <c t="str" r="I118">
         <f t="shared" si="4"/>
-        <v>USPTO</v>
-      </c>
-    </row>
-    <row r="100">
-      <c t="s" s="1" r="A100">
-        <v>599</v>
-      </c>
-      <c s="1" r="B100">
-        <v>17.0</v>
-      </c>
-      <c t="s" s="1" r="C100">
-        <v>600</v>
-      </c>
-      <c t="s" s="2" r="D100">
-        <v>601</v>
-      </c>
-      <c t="s" s="1" r="E100">
-        <v>602</v>
-      </c>
-      <c t="s" s="2" r="F100">
-        <v>603</v>
-      </c>
-      <c s="1" r="G100">
-        <v>49149.0</v>
-      </c>
-      <c t="s" s="2" r="H100">
-        <v>604</v>
-      </c>
-      <c t="str" r="I100">
-        <f t="shared" si="4"/>
-        <v>USCG</v>
-      </c>
-    </row>
-    <row r="101">
-      <c t="s" s="1" r="A101">
-        <v>605</v>
-      </c>
-      <c s="1" r="B101">
-        <v>52.0</v>
-      </c>
-      <c t="s" s="1" r="C101">
-        <v>606</v>
-      </c>
-      <c t="s" s="2" r="D101">
-        <v>607</v>
-      </c>
-      <c t="s" s="1" r="E101">
-        <v>608</v>
-      </c>
-      <c t="s" s="2" r="F101">
-        <v>609</v>
-      </c>
-      <c s="1" r="G101">
-        <v>49126.0</v>
-      </c>
-      <c t="s" s="2" r="H101">
-        <v>610</v>
-      </c>
-      <c t="str" r="I101">
-        <f t="shared" si="4"/>
-        <v>BOP</v>
-      </c>
-    </row>
-    <row r="102">
-      <c t="s" s="1" r="A102">
-        <v>611</v>
-      </c>
-      <c s="1" r="B102">
-        <v>59.0</v>
-      </c>
-      <c t="s" s="1" r="C102">
-        <v>612</v>
-      </c>
-      <c t="s" s="1" r="D102">
-        <v>613</v>
-      </c>
-      <c t="s" s="1" r="E102">
-        <v>614</v>
-      </c>
-      <c t="s" s="2" r="F102">
-        <v>615</v>
-      </c>
-      <c s="1" r="G102">
-        <v>48032.0</v>
-      </c>
-      <c t="s" s="2" r="H102">
-        <v>616</v>
-      </c>
-      <c t="str" r="I102">
-        <f t="shared" si="4"/>
-        <v>EEOC</v>
-      </c>
-    </row>
-    <row r="103">
-      <c t="s" s="1" r="A103">
-        <v>617</v>
-      </c>
-      <c s="1" r="B103">
-        <v>81.0</v>
-      </c>
-      <c t="s" s="1" r="C103">
-        <v>618</v>
-      </c>
-      <c t="s" s="2" r="D103">
-        <v>619</v>
-      </c>
-      <c t="s" s="1" r="E103">
-        <v>620</v>
-      </c>
-      <c t="s" s="2" r="F103">
-        <v>621</v>
-      </c>
-      <c s="1" r="G103">
-        <v>49074.0</v>
-      </c>
-      <c t="s" s="2" r="H103">
-        <v>622</v>
-      </c>
-      <c t="str" r="I103">
-        <f t="shared" si="4"/>
-        <v>AHRQ</v>
-      </c>
-    </row>
-    <row r="104">
-      <c t="s" s="1" r="A104">
-        <v>623</v>
-      </c>
-      <c s="1" r="B104">
-        <v>111.0</v>
-      </c>
-      <c t="s" s="1" r="C104">
-        <v>624</v>
-      </c>
-      <c t="s" s="2" r="D104">
-        <v>625</v>
-      </c>
-      <c t="s" s="1" r="E104">
-        <v>626</v>
-      </c>
-      <c t="s" s="2" r="F104">
-        <v>627</v>
-      </c>
-      <c s="1" r="G104">
-        <v>49586.0</v>
-      </c>
-      <c t="s" s="2" r="H104">
-        <v>628</v>
-      </c>
-      <c t="str" r="I104">
-        <f t="shared" si="4"/>
-        <v>ONDCP</v>
-      </c>
-    </row>
-    <row r="105">
-      <c t="s" s="1" r="A105">
-        <v>629</v>
-      </c>
-      <c s="1" r="B105">
-        <v>6.0</v>
-      </c>
-      <c t="s" s="1" r="C105">
-        <v>630</v>
-      </c>
-      <c t="s" s="2" r="D105">
-        <v>631</v>
-      </c>
-      <c t="s" s="1" r="E105">
-        <v>632</v>
-      </c>
-      <c t="s" s="2" r="F105">
-        <v>633</v>
-      </c>
-      <c s="1" r="G105">
-        <v>49113.0</v>
-      </c>
-      <c t="s" s="2" r="H105">
-        <v>634</v>
-      </c>
-      <c t="str" r="I105">
-        <f t="shared" si="4"/>
-        <v>CFPB</v>
-      </c>
-    </row>
-    <row r="106">
-      <c t="s" s="1" r="A106">
-        <v>635</v>
-      </c>
-      <c s="1" r="B106">
-        <v>50.0</v>
-      </c>
-      <c t="s" s="1" r="C106">
-        <v>636</v>
-      </c>
-      <c t="s" s="2" r="D106">
-        <v>637</v>
-      </c>
-      <c t="s" s="1" r="E106">
-        <v>638</v>
-      </c>
-      <c t="s" s="2" r="F106">
-        <v>639</v>
-      </c>
-      <c s="1" r="G106">
-        <v>52688.0</v>
-      </c>
-      <c t="s" s="2" r="H106">
-        <v>640</v>
-      </c>
-      <c t="str" r="I106">
-        <f t="shared" si="4"/>
-        <v>DEA</v>
-      </c>
-    </row>
-    <row r="107">
-      <c t="s" s="1" r="A107">
-        <v>641</v>
-      </c>
-      <c s="1" r="B107">
-        <v>128.0</v>
-      </c>
-      <c t="s" s="1" r="C107">
-        <v>642</v>
-      </c>
-      <c t="s" s="2" r="D107">
-        <v>643</v>
-      </c>
-      <c t="s" s="1" r="E107">
-        <v>644</v>
-      </c>
-      <c t="s" s="2" r="F107">
-        <v>645</v>
-      </c>
-      <c s="1" r="G107">
-        <v>49691.0</v>
-      </c>
-      <c t="s" s="2" r="H107">
-        <v>646</v>
-      </c>
-      <c t="str" r="I107">
-        <f t="shared" si="4"/>
-        <v>STB</v>
-      </c>
-    </row>
-    <row r="108">
-      <c t="s" s="1" r="A108">
-        <v>647</v>
-      </c>
-      <c s="1" r="B108">
-        <v>98.0</v>
-      </c>
-      <c t="s" s="1" r="C108">
-        <v>648</v>
-      </c>
-      <c t="s" s="2" r="D108">
-        <v>649</v>
-      </c>
-      <c t="s" s="1" r="E108">
-        <v>650</v>
-      </c>
-      <c t="s" s="2" r="F108">
-        <v>651</v>
-      </c>
-      <c s="1" r="G108">
-        <v>52633.0</v>
-      </c>
-      <c t="s" s="2" r="H108">
-        <v>652</v>
-      </c>
-      <c t="str" r="I108">
-        <f t="shared" si="4"/>
-        <v>NCPC</v>
-      </c>
-    </row>
-    <row r="109">
-      <c t="s" s="1" r="A109">
-        <v>653</v>
-      </c>
-      <c s="1" r="B109">
-        <v>89.0</v>
-      </c>
-      <c t="s" s="1" r="C109">
-        <v>654</v>
-      </c>
-      <c t="s" s="1" r="D109">
-        <v>655</v>
-      </c>
-      <c t="s" s="1" r="E109">
-        <v>656</v>
-      </c>
-      <c t="s" s="2" r="F109">
-        <v>657</v>
-      </c>
-      <c s="1" r="G109">
-        <v>49618.0</v>
-      </c>
-      <c t="s" s="2" r="H109">
-        <v>658</v>
-      </c>
-      <c t="str" r="I109">
+        <v>DOD</v>
+      </c>
+    </row>
+    <row r="119">
+      <c t="s" s="1" r="A119">
+        <v>716</v>
+      </c>
+      <c s="1" r="B119">
+        <v>22.0</v>
+      </c>
+      <c t="s" s="1" r="C119">
+        <v>717</v>
+      </c>
+      <c t="s" s="2" r="D119">
+        <v>718</v>
+      </c>
+      <c t="s" s="1" r="E119">
+        <v>719</v>
+      </c>
+      <c t="s" s="2" r="F119">
+        <v>720</v>
+      </c>
+      <c s="1" r="G119">
+        <v>49660.0</v>
+      </c>
+      <c t="s" s="2" r="H119">
+        <v>721</v>
+      </c>
+      <c t="str" r="I119">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="110">
-      <c t="s" s="1" r="A110">
-        <v>659</v>
-      </c>
-      <c s="1" r="B110">
-        <v>136.0</v>
-      </c>
-      <c t="s" s="1" r="C110">
-        <v>660</v>
-      </c>
-      <c t="s" s="2" r="D110">
-        <v>661</v>
-      </c>
-      <c t="s" s="1" r="E110">
-        <v>662</v>
-      </c>
-      <c t="s" s="2" r="F110">
-        <v>663</v>
-      </c>
-      <c s="1" r="G110">
-        <v>49013.0</v>
-      </c>
-      <c t="s" s="2" r="H110">
-        <v>664</v>
-      </c>
-      <c t="str" r="I110">
-        <f t="shared" si="4"/>
-        <v>CPSC</v>
-      </c>
-    </row>
-    <row r="111">
-      <c t="s" s="1" r="A111">
-        <v>665</v>
-      </c>
-      <c s="1" r="B111">
-        <v>94.0</v>
-      </c>
-      <c t="s" s="1" r="C111">
-        <v>666</v>
-      </c>
-      <c t="s" s="1" r="D111">
-        <v>667</v>
-      </c>
-      <c t="s" s="1" r="E111">
-        <v>668</v>
-      </c>
-      <c t="s" s="2" r="F111">
-        <v>669</v>
-      </c>
-      <c s="1" r="G111">
-        <v>52630.0</v>
-      </c>
-      <c t="s" s="2" r="H111">
-        <v>670</v>
-      </c>
-      <c t="str" r="I111">
-        <f t="shared" si="4"/>
-        <v>MSPB</v>
-      </c>
-    </row>
-    <row r="112">
-      <c t="s" s="1" r="A112">
-        <v>671</v>
-      </c>
-      <c s="1" r="B112">
-        <v>28.0</v>
-      </c>
-      <c t="s" s="1" r="C112">
-        <v>672</v>
-      </c>
-      <c t="s" s="2" r="D112">
-        <v>673</v>
-      </c>
-      <c t="s" s="1" r="E112">
-        <v>674</v>
-      </c>
-      <c t="s" s="2" r="F112">
-        <v>675</v>
-      </c>
-      <c s="1" r="G112">
-        <v>49517.0</v>
-      </c>
-      <c t="s" s="2" r="H112">
-        <v>676</v>
-      </c>
-      <c t="str" r="I112">
-        <f t="shared" si="4"/>
-        <v>NIST</v>
-      </c>
-    </row>
-    <row r="113">
-      <c t="s" s="1" r="A113">
-        <v>677</v>
-      </c>
-      <c s="1" r="B113">
-        <v>103.0</v>
-      </c>
-      <c t="s" s="1" r="C113">
-        <v>678</v>
-      </c>
-      <c t="s" s="2" r="D113">
-        <v>679</v>
-      </c>
-      <c t="s" s="1" r="E113">
-        <v>680</v>
-      </c>
-      <c t="s" s="2" r="F113">
-        <v>681</v>
-      </c>
-      <c s="1" r="G113">
-        <v>49523.0</v>
-      </c>
-      <c t="s" s="2" r="H113">
-        <v>682</v>
-      </c>
-      <c t="str" r="I113">
-        <f t="shared" si="4"/>
-        <v>NLRB</v>
-      </c>
-    </row>
-    <row r="114">
-      <c t="s" s="1" r="A114">
-        <v>683</v>
-      </c>
-      <c s="1" r="B114">
-        <v>63.0</v>
-      </c>
-      <c t="s" s="1" r="C114">
-        <v>684</v>
-      </c>
-      <c t="s" s="2" r="D114">
-        <v>685</v>
-      </c>
-      <c t="s" s="1" r="E114">
-        <v>686</v>
-      </c>
-      <c t="s" s="2" r="F114">
-        <v>687</v>
-      </c>
-      <c s="1" r="G114">
-        <v>49041.0</v>
-      </c>
-      <c t="s" s="2" r="H114">
-        <v>688</v>
-      </c>
-      <c t="str" r="I114">
-        <f t="shared" si="4"/>
-        <v>FCC</v>
-      </c>
-    </row>
-    <row r="115">
-      <c t="s" s="1" r="A115">
-        <v>689</v>
-      </c>
-      <c s="1" r="B115">
-        <v>95.0</v>
-      </c>
-      <c t="s" s="1" r="C115">
-        <v>690</v>
-      </c>
-      <c t="s" s="1" r="D115">
-        <v>691</v>
-      </c>
-      <c t="s" s="1" r="E115">
-        <v>692</v>
-      </c>
-      <c t="s" s="2" r="F115">
-        <v>693</v>
-      </c>
-      <c s="1" r="G115">
-        <v>49483.0</v>
-      </c>
-      <c t="s" s="2" r="H115">
-        <v>694</v>
-      </c>
-      <c t="str" r="I115">
-        <f t="shared" si="4"/>
-        <v>NARA</v>
-      </c>
-    </row>
-    <row r="116">
-      <c t="s" s="3" r="A116">
-        <v>695</v>
-      </c>
-      <c s="3" r="B116">
-        <v>75.0</v>
-      </c>
-      <c t="s" s="3" r="C116">
-        <v>696</v>
-      </c>
-      <c t="s" s="4" r="D116">
-        <v>697</v>
-      </c>
-      <c t="s" s="3" r="E116">
-        <v>698</v>
-      </c>
-      <c t="s" s="4" r="F116">
-        <v>699</v>
-      </c>
-      <c s="3" r="G116">
-        <v>49046.0</v>
-      </c>
-      <c t="s" s="4" r="H116">
-        <v>700</v>
-      </c>
-      <c t="s" s="3" r="I116">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="117">
-      <c t="s" s="1" r="A117">
-        <v>702</v>
-      </c>
-      <c s="1" r="B117">
-        <v>54.0</v>
-      </c>
-      <c t="s" s="1" r="C117">
-        <v>703</v>
-      </c>
-      <c t="s" s="2" r="D117">
-        <v>704</v>
-      </c>
-      <c t="s" s="1" r="E117">
-        <v>705</v>
-      </c>
-      <c t="s" s="2" r="F117">
-        <v>706</v>
-      </c>
-      <c s="1" r="G117">
-        <v>49451.0</v>
-      </c>
-      <c t="s" s="2" r="H117">
-        <v>707</v>
-      </c>
-      <c t="str" r="I117">
-        <f ref="I117:I135" t="shared" si="5">iferror(iferror(REGEXEXTRACT(C117,"\((\w+)\)"),REGEXEXTRACT(E117,"\((\w+)\)")),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="118">
-      <c t="s" s="1" r="A118">
-        <v>708</v>
-      </c>
-      <c s="1" r="B118">
-        <v>32.0</v>
-      </c>
-      <c t="s" s="1" r="C118">
-        <v>709</v>
-      </c>
-      <c t="s" s="1" r="D118">
-        <v>710</v>
-      </c>
-      <c t="s" s="1" r="E118">
-        <v>711</v>
-      </c>
-      <c t="s" s="2" r="F118">
-        <v>712</v>
-      </c>
-      <c s="1" r="G118">
-        <v>49229.0</v>
-      </c>
-      <c t="s" s="2" r="H118">
-        <v>713</v>
-      </c>
-      <c t="str" r="I118">
-        <f t="shared" si="5"/>
-        <v>DOD</v>
-      </c>
-    </row>
-    <row r="119">
-      <c t="s" s="1" r="A119">
-        <v>714</v>
-      </c>
-      <c s="1" r="B119">
-        <v>22.0</v>
-      </c>
-      <c t="s" s="1" r="C119">
-        <v>715</v>
-      </c>
-      <c t="s" s="2" r="D119">
-        <v>716</v>
-      </c>
-      <c t="s" s="1" r="E119">
-        <v>717</v>
-      </c>
-      <c t="s" s="2" r="F119">
-        <v>718</v>
-      </c>
-      <c s="1" r="G119">
-        <v>49660.0</v>
-      </c>
-      <c t="s" s="2" r="H119">
-        <v>719</v>
-      </c>
-      <c t="str" r="I119">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
     <row r="120">
       <c t="s" s="1" r="A120">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c s="1" r="B120">
         <v>40.0</v>
       </c>
       <c t="s" s="1" r="C120">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c t="s" s="2" r="D120">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c t="s" s="1" r="E120">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c t="s" s="2" r="F120">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c s="1" r="G120">
         <v>49117.0</v>
       </c>
       <c t="s" s="2" r="H120">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c t="str" r="I120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>BIA</v>
       </c>
     </row>
     <row r="121">
       <c t="s" s="1" r="A121">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c s="1" r="B121">
         <v>100.0</v>
       </c>
       <c t="s" s="1" r="C121">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c t="s" s="2" r="D121">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c t="s" s="1" r="E121">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c t="s" s="2" r="F121">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c s="1" r="G121">
         <v>52634.0</v>
       </c>
       <c t="s" s="2" r="H121">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c t="str" r="I121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>NEA</v>
       </c>
     </row>
     <row r="122">
       <c t="s" s="1" r="A122">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c s="1" r="B122">
         <v>36.0</v>
       </c>
       <c t="s" s="1" r="C122">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c t="s" s="2" r="D122">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c t="s" s="1" r="E122">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c t="s" s="2" r="F122">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c s="1" r="G122">
         <v>49546.0</v>
       </c>
       <c t="s" s="2" r="H122">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c t="str" r="I122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>NSA</v>
       </c>
     </row>
     <row r="123">
       <c t="s" s="1" r="A123">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c s="1" r="B123">
         <v>5.0</v>
       </c>
       <c t="s" s="1" r="C123">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c t="s" s="2" r="D123">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c t="s" s="1" r="E123">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c t="s" s="2" r="F123">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c s="1" r="G123">
         <v>49181.0</v>
       </c>
       <c t="s" s="2" r="H123">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c t="str" r="I123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CEQ</v>
       </c>
     </row>
     <row r="124">
       <c t="s" s="1" r="A124">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c s="1" r="B124">
         <v>43.0</v>
       </c>
       <c t="s" s="1" r="C124">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c t="s" s="2" r="D124">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c t="s" s="1" r="E124">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c t="s" s="2" r="F124">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c s="1" r="G124">
         <v>49128.0</v>
       </c>
       <c t="s" s="2" r="H124">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c t="str" r="I124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>USBR</v>
       </c>
     </row>
     <row r="125">
       <c t="s" s="1" r="A125">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c s="1" r="B125">
         <v>151.0</v>
       </c>
       <c t="s" s="1" r="C125">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c t="s" s="2" r="D125">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c t="s" s="1" r="E125">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c t="s" s="2" r="F125">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c s="1" r="G125">
         <v>52645.0</v>
       </c>
       <c t="s" s="2" r="H125">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c t="str" r="I125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>NRC</v>
       </c>
     </row>
     <row r="126">
       <c t="s" s="1" r="A126">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c s="1" r="B126">
         <v>55.0</v>
       </c>
       <c t="s" s="1" r="C126">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c t="s" s="1" r="D126">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c t="s" s="1" r="E126">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c t="s" s="2" r="F126">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c s="1" r="G126">
         <v>49035.0</v>
       </c>
       <c t="s" s="2" r="H126">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c t="str" r="I126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>DOT</v>
       </c>
     </row>
     <row r="127">
       <c t="s" s="1" r="A127">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c s="1" r="B127">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="C127">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c t="s" s="2" r="D127">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c t="s" s="1" r="E127">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c t="s" s="2" r="F127">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c s="1" r="G127">
         <v>52584.0</v>
       </c>
       <c t="s" s="2" r="H127">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c t="str" r="I127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ABMC</v>
       </c>
     </row>
     <row r="128">
       <c t="s" s="1" r="A128">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c s="1" r="B128">
         <v>44.0</v>
       </c>
       <c t="s" s="1" r="C128">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c t="s" s="2" r="D128">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c t="s" s="1" r="E128">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c t="s" s="2" r="F128">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c s="1" r="G128">
         <v>85146.0</v>
       </c>
       <c t="s" s="2" r="H128">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c t="str" r="I128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>BSEE</v>
       </c>
     </row>
     <row r="129">
       <c t="s" s="1" r="A129">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c s="1" r="B129">
         <v>119.0</v>
       </c>
       <c t="s" s="1" r="C129">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c t="s" s="1" r="D129">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c t="s" s="1" r="E129">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c t="s" s="2" r="F129">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c s="1" r="G129">
         <v>52652.0</v>
       </c>
       <c t="s" s="2" r="H129">
-        <v>779</v>
-      </c>
-      <c t="str" r="I129">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>781</v>
+      </c>
+      <c t="s" s="1" r="I129">
+        <v>782</v>
       </c>
     </row>
     <row r="130">
       <c t="s" s="1" r="A130">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c s="1" r="B130">
         <v>117.0</v>
       </c>
       <c t="s" s="1" r="C130">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c t="s" s="2" r="D130">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c t="s" s="1" r="E130">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c t="s" s="2" r="F130">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c s="1" r="G130">
         <v>49590.0</v>
       </c>
       <c t="s" s="2" r="H130">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c t="str" r="I130">
-        <f t="shared" si="5"/>
+        <f ref="I130:I135" t="shared" si="5">iferror(iferror(REGEXEXTRACT(C130,"\((\w+)\)"),REGEXEXTRACT(E130,"\((\w+)\)")),"")</f>
         <v>OSTP</v>
       </c>
     </row>
     <row r="131">
       <c t="s" s="1" r="A131">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c s="1" r="B131">
         <v>57.0</v>
       </c>
       <c t="s" s="1" r="C131">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c t="s" s="2" r="D131">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c t="s" s="1" r="E131">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c t="s" s="2" r="F131">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c s="1" r="G131">
         <v>48081.0</v>
       </c>
       <c t="s" s="2" r="H131">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c t="str" r="I131">
         <f t="shared" si="5"/>
@@ -7176,28 +7196,28 @@
     </row>
     <row r="132">
       <c t="s" s="1" r="A132">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c s="1" r="B132">
         <v>13.0</v>
       </c>
       <c t="s" s="1" r="C132">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c t="s" s="2" r="D132">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c t="s" s="1" r="E132">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c t="s" s="2" r="F132">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c s="1" r="G132">
         <v>52591.0</v>
       </c>
       <c t="s" s="2" r="H132">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c t="str" r="I132">
         <f t="shared" si="5"/>
@@ -7206,28 +7226,28 @@
     </row>
     <row r="133">
       <c t="s" s="1" r="A133">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c s="1" r="B133">
         <v>41.0</v>
       </c>
       <c t="s" s="1" r="C133">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c t="s" s="2" r="D133">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c t="s" s="1" r="E133">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c t="s" s="2" r="F133">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c s="1" r="G133">
         <v>49125.0</v>
       </c>
       <c t="s" s="2" r="H133">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c t="str" r="I133">
         <f t="shared" si="5"/>
@@ -7236,28 +7256,28 @@
     </row>
     <row r="134">
       <c t="s" s="1" r="A134">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c s="1" r="B134">
         <v>30.0</v>
       </c>
       <c t="s" s="1" r="C134">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c t="s" s="2" r="D134">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c t="s" s="1" r="E134">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c t="s" s="2" r="F134">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c s="1" r="G134">
         <v>49530.0</v>
       </c>
       <c t="s" s="2" r="H134">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c t="str" r="I134">
         <f t="shared" si="5"/>
@@ -7266,28 +7286,28 @@
     </row>
     <row r="135">
       <c t="s" s="1" r="A135">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c s="1" r="B135">
         <v>140.0</v>
       </c>
       <c t="s" s="1" r="C135">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c t="s" s="2" r="D135">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c t="s" s="1" r="E135">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c t="s" s="2" r="F135">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c s="1" r="G135">
         <v>48029.0</v>
       </c>
       <c t="s" s="2" r="H135">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c t="str" r="I135">
         <f t="shared" si="5"/>
@@ -7296,76 +7316,76 @@
     </row>
     <row r="136">
       <c t="s" s="3" r="A136">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c s="3" r="B136">
         <v>9.0</v>
       </c>
       <c t="s" s="3" r="C136">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c t="s" s="4" r="D136">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c t="s" s="3" r="E136">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c t="s" s="4" r="F136">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c s="3" r="G136">
         <v>91390.0</v>
       </c>
       <c s="7" r="H136"/>
       <c t="s" s="3" r="I136">
-        <v>821</v>
+        <v>824</v>
       </c>
     </row>
     <row r="137">
       <c t="s" s="1" r="A137">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c s="1" r="B137">
         <v>12.0</v>
       </c>
       <c t="s" s="1" r="C137">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c t="s" s="2" r="D137">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c t="s" s="8" r="E137">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c t="s" s="2" r="F137">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c s="1" r="G137">
         <v>49157.0</v>
       </c>
       <c t="str" r="I137">
-        <f ref="I137:I163" t="shared" si="6">iferror(iferror(REGEXEXTRACT(C137,"\((\w+)\)"),REGEXEXTRACT(E137,"\((\w+)\)")),"")</f>
+        <f ref="I137:I153" t="shared" si="6">iferror(iferror(REGEXEXTRACT(C137,"\((\w+)\)"),REGEXEXTRACT(E137,"\((\w+)\)")),"")</f>
         <v>CPPBSD</v>
       </c>
     </row>
     <row r="138">
       <c t="s" s="1" r="A138">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c s="1" r="B138">
         <v>14.0</v>
       </c>
       <c t="s" s="1" r="C138">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c t="s" s="2" r="D138">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c t="s" s="1" r="E138">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c t="s" s="2" r="F138">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c s="1" r="G138">
         <v>49191.0</v>
@@ -7377,22 +7397,22 @@
     </row>
     <row r="139">
       <c t="s" s="1" r="A139">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c s="1" r="B139">
         <v>18.0</v>
       </c>
       <c t="s" s="1" r="C139">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c t="s" s="2" r="D139">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c t="s" s="9" r="E139">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c t="s" s="2" r="F139">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c s="1" r="G139">
         <v>55927.0</v>
@@ -7404,22 +7424,22 @@
     </row>
     <row r="140">
       <c t="s" s="1" r="A140">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c s="1" r="B140">
         <v>21.0</v>
       </c>
       <c t="s" s="1" r="C140">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c t="s" s="2" r="D140">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c t="s" s="1" r="E140">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c t="s" s="2" r="F140">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c s="1" r="G140">
         <v>49711.0</v>
@@ -7431,22 +7451,22 @@
     </row>
     <row r="141">
       <c t="s" s="1" r="A141">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c s="1" r="B141">
         <v>25.0</v>
       </c>
       <c t="s" s="1" r="C141">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c t="s" s="2" r="D141">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c t="s" s="1" r="E141">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c t="s" s="2" r="F141">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c s="1" r="G141">
         <v>48005.0</v>
@@ -7458,28 +7478,28 @@
     </row>
     <row r="142">
       <c t="s" s="1" r="A142">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c s="1" r="B142">
         <v>33.0</v>
       </c>
       <c t="s" s="1" r="C142">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c t="s" s="2" r="D142">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c t="s" s="1" r="E142">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c t="s" s="2" r="F142">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c t="s" s="1" r="G142">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c t="s" s="1" r="H142">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c t="str" r="I142">
         <f t="shared" si="6"/>
@@ -7488,22 +7508,22 @@
     </row>
     <row r="143">
       <c t="s" s="1" r="A143">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c s="1" r="B143">
         <v>48.0</v>
       </c>
       <c t="s" s="1" r="C143">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c t="s" s="2" r="D143">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c t="s" s="1" r="E143">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c t="s" s="2" r="F143">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c t="str" r="I143">
         <f t="shared" si="6"/>
@@ -7512,22 +7532,22 @@
     </row>
     <row r="144">
       <c t="s" s="1" r="A144">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c s="1" r="B144">
         <v>61.0</v>
       </c>
       <c t="s" s="1" r="C144">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c t="s" s="2" r="D144">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c t="s" s="1" r="E144">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c t="s" s="2" r="F144">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c s="1" r="G144">
         <v>52603.0</v>
@@ -7539,22 +7559,22 @@
     </row>
     <row r="145">
       <c t="s" s="1" r="A145">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c s="1" r="B145">
         <v>74.0</v>
       </c>
       <c t="s" s="1" r="C145">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c t="s" s="2" r="D145">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c t="s" s="1" r="E145">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c t="s" s="2" r="F145">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c t="str" r="I145">
         <f t="shared" si="6"/>
@@ -7563,22 +7583,22 @@
     </row>
     <row r="146">
       <c t="s" s="1" r="A146">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c s="1" r="B146">
         <v>80.0</v>
       </c>
       <c t="s" s="1" r="C146">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c t="s" s="2" r="D146">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c t="s" s="1" r="E146">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c t="s" s="2" r="F146">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c t="str" r="I146">
         <f t="shared" si="6"/>
@@ -7587,22 +7607,22 @@
     </row>
     <row r="147">
       <c t="s" s="1" r="A147">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c s="1" r="B147">
         <v>83.0</v>
       </c>
       <c t="s" s="1" r="C147">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c t="s" s="2" r="D147">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c t="s" s="1" r="E147">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c t="s" s="2" r="F147">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c s="1" r="G147">
         <v>49134.0</v>
@@ -7614,22 +7634,22 @@
     </row>
     <row r="148">
       <c t="s" s="1" r="A148">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c s="1" r="B148">
         <v>88.0</v>
       </c>
       <c t="s" s="1" r="C148">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c t="s" s="2" r="D148">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c t="s" s="1" r="E148">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c t="s" s="2" r="F148">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c s="1" r="G148">
         <v>49687.0</v>
@@ -7641,22 +7661,22 @@
     </row>
     <row r="149">
       <c t="s" s="1" r="A149">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c s="1" r="B149">
         <v>97.0</v>
       </c>
       <c t="s" s="1" r="C149">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c t="s" s="2" r="D149">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c t="s" s="1" r="E149">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c t="s" s="2" r="F149">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c t="str" r="I149">
         <f t="shared" si="6"/>
@@ -7665,22 +7685,22 @@
     </row>
     <row r="150">
       <c t="s" s="1" r="A150">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c s="1" r="B150">
         <v>105.0</v>
       </c>
       <c t="s" s="1" r="C150">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c t="s" s="2" r="D150">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c t="s" s="1" r="E150">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c t="s" s="2" r="F150">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c s="1" r="G150">
         <v>49084.0</v>
@@ -7692,22 +7712,22 @@
     </row>
     <row r="151">
       <c t="s" s="1" r="A151">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c s="1" r="B151">
         <v>112.0</v>
       </c>
       <c t="s" s="1" r="C151">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c t="s" s="2" r="D151">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c t="s" s="1" r="E151">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c t="s" s="2" r="F151">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c t="str" r="I151">
         <f t="shared" si="6"/>
@@ -7716,22 +7736,22 @@
     </row>
     <row r="152">
       <c t="s" s="1" r="A152">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c s="1" r="B152">
         <v>121.0</v>
       </c>
       <c t="s" s="1" r="C152">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c t="s" s="2" r="D152">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c t="s" s="1" r="E152">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c t="s" s="2" r="F152">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c t="str" r="I152">
         <f t="shared" si="6"/>
@@ -7740,22 +7760,22 @@
     </row>
     <row r="153">
       <c t="s" s="1" r="A153">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c s="1" r="B153">
         <v>124.0</v>
       </c>
       <c t="s" s="1" r="C153">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c t="s" s="2" r="D153">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c t="s" s="1" r="E153">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c t="s" s="2" r="F153">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c t="str" r="I153">
         <f t="shared" si="6"/>
@@ -7763,265 +7783,265 @@
       </c>
     </row>
     <row r="154">
-      <c t="s" s="1" r="A154">
-        <v>909</v>
-      </c>
-      <c s="1" r="B154">
+      <c t="s" s="3" r="A154">
+        <v>912</v>
+      </c>
+      <c s="3" r="B154">
         <v>129.0</v>
       </c>
-      <c t="s" s="1" r="C154">
-        <v>910</v>
-      </c>
-      <c t="s" s="1" r="D154">
-        <v>911</v>
-      </c>
-      <c t="s" s="1" r="E154">
-        <v>912</v>
-      </c>
-      <c t="s" s="2" r="F154">
+      <c t="s" s="3" r="C154">
         <v>913</v>
       </c>
-      <c s="1" r="G154">
+      <c t="s" s="3" r="D154">
+        <v>914</v>
+      </c>
+      <c t="s" s="3" r="E154">
+        <v>915</v>
+      </c>
+      <c t="s" s="4" r="F154">
+        <v>916</v>
+      </c>
+      <c s="3" r="G154">
         <v>49034.0</v>
       </c>
-      <c t="str" r="I154">
-        <f t="shared" si="6"/>
-        <v/>
+      <c s="7" r="H154"/>
+      <c t="s" s="3" r="I154">
+        <v>917</v>
       </c>
     </row>
     <row r="155">
       <c t="s" s="1" r="A155">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c s="1" r="B155">
         <v>132.0</v>
       </c>
       <c t="s" s="1" r="C155">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c t="s" s="2" r="D155">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c t="s" s="1" r="E155">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c t="s" s="2" r="F155">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c s="1" r="G155">
         <v>48126.0</v>
       </c>
       <c t="str" r="I155">
-        <f t="shared" si="6"/>
+        <f ref="I155:I162" t="shared" si="7">iferror(iferror(REGEXEXTRACT(C155,"\((\w+)\)"),REGEXEXTRACT(E155,"\((\w+)\)")),"")</f>
         <v>OCC</v>
       </c>
     </row>
     <row r="156">
       <c t="s" s="1" r="A156">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c s="1" r="B156">
         <v>133.0</v>
       </c>
       <c t="s" s="1" r="C156">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c t="s" s="2" r="D156">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c t="s" s="1" r="E156">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c t="s" s="2" r="F156">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c t="str" r="I156">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FINCEN</v>
       </c>
     </row>
     <row r="157">
       <c t="s" s="1" r="A157">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c s="1" r="B157">
         <v>141.0</v>
       </c>
       <c t="s" s="1" r="C157">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c t="s" s="2" r="D157">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c t="s" s="1" r="E157">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c t="s" s="10" r="F157">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c s="1" r="G157">
         <v>52693.0</v>
       </c>
       <c t="str" r="I157">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DOLETA</v>
       </c>
     </row>
     <row r="158">
       <c t="s" s="1" r="A158">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c s="1" r="B158">
         <v>142.0</v>
       </c>
       <c t="s" s="1" r="C158">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c t="s" s="2" r="D158">
-        <v>931</v>
+        <v>935</v>
       </c>
       <c t="s" s="1" r="E158">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c t="s" s="10" r="F158">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c s="1" r="G158">
         <v>49462.0</v>
       </c>
       <c t="str" r="I158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>MSHA</v>
       </c>
     </row>
     <row r="159">
       <c t="s" s="1" r="A159">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c s="1" r="B159">
         <v>149.0</v>
       </c>
       <c t="s" s="1" r="C159">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c t="s" s="2" r="D159">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c t="s" s="1" r="E159">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c t="s" s="2" r="F159">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c t="str" r="I159">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>IBWC</v>
       </c>
     </row>
     <row r="160">
       <c t="s" s="1" r="A160">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c s="1" r="B160">
         <v>150.0</v>
       </c>
       <c t="s" s="1" r="C160">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c t="s" s="2" r="D160">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c t="s" s="1" r="E160">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c t="s" s="2" r="F160">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c s="1" r="G160">
         <v>49712.0</v>
       </c>
       <c t="str" r="I160">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>USITC</v>
       </c>
     </row>
     <row r="161">
       <c t="s" s="1" r="A161">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c s="1" r="B161">
         <v>153.0</v>
       </c>
       <c t="s" s="1" r="C161">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c t="s" s="2" r="D161">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c t="s" s="1" r="E161">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c t="s" s="2" r="F161">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c s="1" r="G161"/>
       <c t="str" r="I161">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="162">
       <c t="s" s="1" r="A162">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c s="1" r="B162">
         <v>154.0</v>
       </c>
       <c t="s" s="1" r="C162">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c t="s" s="2" r="D162">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c t="s" s="1" r="E162">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c t="s" s="10" r="F162">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c s="1" r="G162">
         <v>49721.0</v>
       </c>
       <c t="str" r="I162">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>USTDA</v>
       </c>
     </row>
     <row r="163">
-      <c t="s" s="1" r="A163">
-        <v>954</v>
-      </c>
-      <c s="1" r="B163">
+      <c t="s" s="3" r="A163">
+        <v>958</v>
+      </c>
+      <c s="3" r="B163">
         <v>155.0</v>
       </c>
-      <c t="s" s="1" r="C163">
-        <v>955</v>
-      </c>
-      <c t="s" s="2" r="D163">
-        <v>956</v>
-      </c>
-      <c t="s" s="1" r="E163">
-        <v>957</v>
-      </c>
-      <c t="s" s="10" r="F163">
-        <v>958</v>
-      </c>
-      <c s="1" r="G163">
+      <c t="s" s="3" r="C163">
+        <v>959</v>
+      </c>
+      <c t="s" s="4" r="D163">
+        <v>960</v>
+      </c>
+      <c t="s" s="3" r="E163">
+        <v>961</v>
+      </c>
+      <c t="s" s="11" r="F163">
+        <v>962</v>
+      </c>
+      <c s="3" r="G163">
         <v>49724.0</v>
       </c>
-      <c t="str" r="I163">
-        <f t="shared" si="6"/>
-        <v/>
+      <c s="7" r="H163"/>
+      <c t="s" s="3" r="I163">
+        <v>963</v>
       </c>
     </row>
   </sheetData>
@@ -8481,46 +8501,46 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>959</v>
+        <v>964</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>960</v>
+        <v>965</v>
       </c>
       <c t="s" s="1" r="C1">
-        <v>961</v>
+        <v>966</v>
       </c>
       <c t="s" s="1" r="D1">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c t="s" s="1" r="E1">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c t="s" s="1" r="F1">
-        <v>964</v>
+        <v>969</v>
       </c>
       <c t="s" s="1" r="G1">
-        <v>965</v>
-      </c>
-      <c s="11" r="H1"/>
+        <v>970</v>
+      </c>
+      <c s="12" r="H1"/>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>966</v>
+        <v>971</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>967</v>
+        <v>972</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>968</v>
+        <v>973</v>
       </c>
       <c t="s" s="2" r="D2">
-        <v>969</v>
+        <v>974</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>970</v>
+        <v>975</v>
       </c>
       <c t="s" s="1" r="F2">
-        <v>971</v>
+        <v>976</v>
       </c>
       <c t="str" r="G2">
         <f ref="G2:G12" t="shared" si="1">iferror(iferror(REGEXEXTRACT(A2,"\((\w+)\)"),REGEXEXTRACT(C2,"\((\w+)\)")),"")</f>
@@ -8529,16 +8549,16 @@
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>972</v>
+        <v>977</v>
       </c>
       <c t="s" s="2" r="B3">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c t="s" s="2" r="D3">
-        <v>975</v>
+        <v>980</v>
       </c>
       <c t="str" r="G3">
         <f t="shared" si="1"/>
@@ -8547,16 +8567,16 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>976</v>
+        <v>981</v>
       </c>
       <c t="s" s="2" r="B4">
-        <v>977</v>
+        <v>982</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>978</v>
+        <v>983</v>
       </c>
       <c t="s" s="2" r="D4">
-        <v>979</v>
+        <v>984</v>
       </c>
       <c t="str" r="G4">
         <f t="shared" si="1"/>
@@ -8565,16 +8585,16 @@
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>980</v>
+        <v>985</v>
       </c>
       <c t="s" s="2" r="B5">
-        <v>981</v>
+        <v>986</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>982</v>
+        <v>987</v>
       </c>
       <c t="s" s="2" r="D5">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c t="str" r="G5">
         <f t="shared" si="1"/>
@@ -8583,16 +8603,16 @@
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>984</v>
+        <v>989</v>
       </c>
       <c t="s" s="2" r="B6">
-        <v>985</v>
+        <v>990</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>986</v>
+        <v>991</v>
       </c>
       <c t="s" s="2" r="D6">
-        <v>987</v>
+        <v>992</v>
       </c>
       <c t="str" r="G6">
         <f t="shared" si="1"/>
@@ -8601,16 +8621,16 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c t="s" s="2" r="B7">
-        <v>989</v>
+        <v>994</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>990</v>
+        <v>995</v>
       </c>
       <c t="s" s="2" r="D7">
-        <v>991</v>
+        <v>996</v>
       </c>
       <c t="str" r="G7">
         <f t="shared" si="1"/>
@@ -8619,16 +8639,16 @@
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>992</v>
+        <v>997</v>
       </c>
       <c t="s" s="2" r="B8">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c t="s" s="2" r="D8">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c t="str" r="G8">
         <f t="shared" si="1"/>
@@ -8637,16 +8657,16 @@
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c t="s" s="2" r="B9">
-        <v>997</v>
+        <v>1002</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c t="s" s="2" r="D9">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c t="str" r="G9">
         <f t="shared" si="1"/>
@@ -8655,16 +8675,16 @@
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>1000</v>
+        <v>1005</v>
       </c>
       <c t="s" s="2" r="B10">
-        <v>1001</v>
+        <v>1006</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c t="s" s="2" r="D10">
-        <v>1003</v>
+        <v>1008</v>
       </c>
       <c t="str" r="G10">
         <f t="shared" si="1"/>
@@ -8673,16 +8693,16 @@
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c t="s" s="2" r="B11">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c t="s" s="2" r="D11">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c t="str" r="G11">
         <f t="shared" si="1"/>
@@ -8691,16 +8711,16 @@
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>1008</v>
+        <v>1013</v>
       </c>
       <c t="s" s="2" r="B12">
-        <v>1009</v>
+        <v>1014</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>1010</v>
+        <v>1015</v>
       </c>
       <c t="s" s="2" r="D12">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c s="1" r="E12"/>
       <c t="str" r="G12">

</xml_diff>

<commit_message>
fixed dup on HUD
</commit_message>
<xml_diff>
--- a/contacts/usagov-data/foiaHub-usaContacts-matches.xlsx
+++ b/contacts/usagov-data/foiaHub-usaContacts-matches.xlsx
@@ -2020,7 +2020,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Department of Housing and Urban Development</t>
+    <t>Policy Development and Research </t>
   </si>
   <si>
     <t>None</t>
@@ -2033,6 +2033,9 @@
   </si>
   <si>
     <t>http://www.usa.gov/directory/federal/policy-development-and-research.shtml</t>
+  </si>
+  <si>
+    <t>HUDUSER</t>
   </si>
   <si>
     <t>No</t>
@@ -3107,7 +3110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -3130,11 +3133,15 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF545454"/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF545454"/>
     </font>
     <font>
       <u/>
@@ -3147,7 +3154,7 @@
       <color rgb="FF1155CC"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3164,6 +3171,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3205,7 +3218,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -3225,17 +3238,26 @@
     <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="5">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="6">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="7">
+      <alignment/>
+    </xf>
     <xf fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="6" applyFill="1">
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="7">
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="7">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8">
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="9">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="9">
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="10">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
@@ -6202,7 +6224,7 @@
         <v>594</v>
       </c>
       <c t="str" r="I98">
-        <f ref="I98:I115" t="shared" si="3">iferror(iferror(REGEXEXTRACT(C98,"\((\w+)\)"),REGEXEXTRACT(E98,"\((\w+)\)")),"")</f>
+        <f ref="I98:I108" t="shared" si="3">iferror(iferror(REGEXEXTRACT(C98,"\((\w+)\)"),REGEXEXTRACT(E98,"\((\w+)\)")),"")</f>
         <v>GSA</v>
       </c>
     </row>
@@ -6507,1541 +6529,1540 @@
       </c>
     </row>
     <row r="109">
-      <c t="s" s="1" r="A109">
+      <c t="s" s="7" r="A109">
         <v>655</v>
       </c>
-      <c s="1" r="B109">
+      <c s="7" r="B109">
         <v>89.0</v>
       </c>
-      <c t="s" s="1" r="C109">
+      <c t="s" s="7" r="C109">
         <v>656</v>
       </c>
-      <c t="s" s="1" r="D109">
+      <c t="s" s="7" r="D109">
         <v>657</v>
       </c>
-      <c t="s" s="1" r="E109">
+      <c t="s" s="7" r="E109">
         <v>658</v>
       </c>
-      <c t="s" s="2" r="F109">
+      <c t="s" s="8" r="F109">
         <v>659</v>
       </c>
-      <c s="1" r="G109">
+      <c s="9" r="G109">
         <v>49618.0</v>
       </c>
-      <c t="s" s="2" r="H109">
+      <c t="s" s="8" r="H109">
         <v>660</v>
       </c>
-      <c t="str" r="I109">
-        <f t="shared" si="3"/>
-        <v/>
+      <c t="s" s="9" r="I109">
+        <v>661</v>
       </c>
     </row>
     <row r="110">
       <c t="s" s="1" r="A110">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c s="1" r="B110">
         <v>136.0</v>
       </c>
       <c t="s" s="1" r="C110">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c t="s" s="2" r="D110">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c t="s" s="1" r="E110">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c t="s" s="2" r="F110">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c s="1" r="G110">
         <v>49013.0</v>
       </c>
       <c t="s" s="2" r="H110">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c t="str" r="I110">
-        <f t="shared" si="3"/>
+        <f ref="I110:I115" t="shared" si="4">iferror(iferror(REGEXEXTRACT(C110,"\((\w+)\)"),REGEXEXTRACT(E110,"\((\w+)\)")),"")</f>
         <v>CPSC</v>
       </c>
     </row>
     <row r="111">
       <c t="s" s="1" r="A111">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c s="1" r="B111">
         <v>94.0</v>
       </c>
       <c t="s" s="1" r="C111">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c t="s" s="1" r="D111">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c t="s" s="1" r="E111">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c t="s" s="2" r="F111">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c s="1" r="G111">
         <v>52630.0</v>
       </c>
       <c t="s" s="2" r="H111">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c t="str" r="I111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>MSPB</v>
       </c>
     </row>
     <row r="112">
       <c t="s" s="1" r="A112">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c s="1" r="B112">
         <v>28.0</v>
       </c>
       <c t="s" s="1" r="C112">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c t="s" s="2" r="D112">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c t="s" s="1" r="E112">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c t="s" s="2" r="F112">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c s="1" r="G112">
         <v>49517.0</v>
       </c>
       <c t="s" s="2" r="H112">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c t="str" r="I112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>NIST</v>
       </c>
     </row>
     <row r="113">
       <c t="s" s="1" r="A113">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c s="1" r="B113">
         <v>103.0</v>
       </c>
       <c t="s" s="1" r="C113">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c t="s" s="2" r="D113">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c t="s" s="1" r="E113">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c t="s" s="2" r="F113">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c s="1" r="G113">
         <v>49523.0</v>
       </c>
       <c t="s" s="2" r="H113">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c t="str" r="I113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>NLRB</v>
       </c>
     </row>
     <row r="114">
       <c t="s" s="1" r="A114">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c s="1" r="B114">
         <v>63.0</v>
       </c>
       <c t="s" s="1" r="C114">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c t="s" s="2" r="D114">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c t="s" s="1" r="E114">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c t="s" s="2" r="F114">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c s="1" r="G114">
         <v>49041.0</v>
       </c>
       <c t="s" s="2" r="H114">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c t="str" r="I114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>FCC</v>
       </c>
     </row>
     <row r="115">
       <c t="s" s="1" r="A115">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c s="1" r="B115">
         <v>95.0</v>
       </c>
       <c t="s" s="1" r="C115">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c t="s" s="1" r="D115">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c t="s" s="1" r="E115">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c t="s" s="2" r="F115">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c s="1" r="G115">
         <v>49483.0</v>
       </c>
       <c t="s" s="2" r="H115">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c t="str" r="I115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>NARA</v>
       </c>
     </row>
     <row r="116">
       <c t="s" s="3" r="A116">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c s="3" r="B116">
         <v>75.0</v>
       </c>
       <c t="s" s="3" r="C116">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c t="s" s="4" r="D116">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c t="s" s="3" r="E116">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c t="s" s="4" r="F116">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c s="3" r="G116">
         <v>49046.0</v>
       </c>
       <c t="s" s="4" r="H116">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c t="s" s="3" r="I116">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="117">
       <c t="s" s="1" r="A117">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c s="1" r="B117">
         <v>54.0</v>
       </c>
       <c t="s" s="1" r="C117">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c t="s" s="2" r="D117">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c t="s" s="1" r="E117">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c t="s" s="2" r="F117">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c s="1" r="G117">
         <v>49451.0</v>
       </c>
       <c t="s" s="2" r="H117">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c t="str" r="I117">
-        <f ref="I117:I128" t="shared" si="4">iferror(iferror(REGEXEXTRACT(C117,"\((\w+)\)"),REGEXEXTRACT(E117,"\((\w+)\)")),"")</f>
+        <f ref="I117:I128" t="shared" si="5">iferror(iferror(REGEXEXTRACT(C117,"\((\w+)\)"),REGEXEXTRACT(E117,"\((\w+)\)")),"")</f>
         <v/>
       </c>
     </row>
     <row r="118">
       <c t="s" s="1" r="A118">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c s="1" r="B118">
         <v>32.0</v>
       </c>
       <c t="s" s="1" r="C118">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c t="s" s="1" r="D118">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c t="s" s="1" r="E118">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c t="s" s="2" r="F118">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c s="1" r="G118">
         <v>49229.0</v>
       </c>
       <c t="s" s="2" r="H118">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c t="str" r="I118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DOD</v>
       </c>
     </row>
     <row r="119">
       <c t="s" s="1" r="A119">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c s="1" r="B119">
         <v>22.0</v>
       </c>
       <c t="s" s="1" r="C119">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c t="s" s="2" r="D119">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c t="s" s="1" r="E119">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c t="s" s="2" r="F119">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c s="1" r="G119">
         <v>49660.0</v>
       </c>
       <c t="s" s="2" r="H119">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c t="str" r="I119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="120">
       <c t="s" s="1" r="A120">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c s="1" r="B120">
         <v>40.0</v>
       </c>
       <c t="s" s="1" r="C120">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c t="s" s="2" r="D120">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c t="s" s="1" r="E120">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c t="s" s="2" r="F120">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c s="1" r="G120">
         <v>49117.0</v>
       </c>
       <c t="s" s="2" r="H120">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c t="str" r="I120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BIA</v>
       </c>
     </row>
     <row r="121">
       <c t="s" s="1" r="A121">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c s="1" r="B121">
         <v>100.0</v>
       </c>
       <c t="s" s="1" r="C121">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c t="s" s="2" r="D121">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c t="s" s="1" r="E121">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c t="s" s="2" r="F121">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c s="1" r="G121">
         <v>52634.0</v>
       </c>
       <c t="s" s="2" r="H121">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c t="str" r="I121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>NEA</v>
       </c>
     </row>
     <row r="122">
       <c t="s" s="1" r="A122">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c s="1" r="B122">
         <v>36.0</v>
       </c>
       <c t="s" s="1" r="C122">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c t="s" s="2" r="D122">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c t="s" s="1" r="E122">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c t="s" s="2" r="F122">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c s="1" r="G122">
         <v>49546.0</v>
       </c>
       <c t="s" s="2" r="H122">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c t="str" r="I122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>NSA</v>
       </c>
     </row>
     <row r="123">
       <c t="s" s="1" r="A123">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c s="1" r="B123">
         <v>5.0</v>
       </c>
       <c t="s" s="1" r="C123">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c t="s" s="2" r="D123">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c t="s" s="1" r="E123">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c t="s" s="2" r="F123">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c s="1" r="G123">
         <v>49181.0</v>
       </c>
       <c t="s" s="2" r="H123">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c t="str" r="I123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CEQ</v>
       </c>
     </row>
     <row r="124">
       <c t="s" s="1" r="A124">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c s="1" r="B124">
         <v>43.0</v>
       </c>
       <c t="s" s="1" r="C124">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c t="s" s="2" r="D124">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c t="s" s="1" r="E124">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c t="s" s="2" r="F124">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c s="1" r="G124">
         <v>49128.0</v>
       </c>
       <c t="s" s="2" r="H124">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c t="str" r="I124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>USBR</v>
       </c>
     </row>
     <row r="125">
       <c t="s" s="1" r="A125">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c s="1" r="B125">
         <v>151.0</v>
       </c>
       <c t="s" s="1" r="C125">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c t="s" s="2" r="D125">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c t="s" s="1" r="E125">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c t="s" s="2" r="F125">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c s="1" r="G125">
         <v>52645.0</v>
       </c>
       <c t="s" s="2" r="H125">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c t="str" r="I125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>NRC</v>
       </c>
     </row>
     <row r="126">
       <c t="s" s="1" r="A126">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c s="1" r="B126">
         <v>55.0</v>
       </c>
       <c t="s" s="1" r="C126">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c t="s" s="1" r="D126">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c t="s" s="1" r="E126">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c t="s" s="2" r="F126">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c s="1" r="G126">
         <v>49035.0</v>
       </c>
       <c t="s" s="2" r="H126">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c t="str" r="I126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DOT</v>
       </c>
     </row>
     <row r="127">
       <c t="s" s="1" r="A127">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c s="1" r="B127">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="C127">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c t="s" s="2" r="D127">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c t="s" s="1" r="E127">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c t="s" s="2" r="F127">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c s="1" r="G127">
         <v>52584.0</v>
       </c>
       <c t="s" s="2" r="H127">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c t="str" r="I127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ABMC</v>
       </c>
     </row>
     <row r="128">
       <c t="s" s="1" r="A128">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c s="1" r="B128">
         <v>44.0</v>
       </c>
       <c t="s" s="1" r="C128">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c t="s" s="2" r="D128">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c t="s" s="1" r="E128">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c t="s" s="2" r="F128">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c s="1" r="G128">
         <v>85146.0</v>
       </c>
       <c t="s" s="2" r="H128">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c t="str" r="I128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BSEE</v>
       </c>
     </row>
     <row r="129">
       <c t="s" s="1" r="A129">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c s="1" r="B129">
         <v>119.0</v>
       </c>
       <c t="s" s="1" r="C129">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c t="s" s="1" r="D129">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c t="s" s="1" r="E129">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c t="s" s="2" r="F129">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c s="1" r="G129">
         <v>52652.0</v>
       </c>
       <c t="s" s="2" r="H129">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c t="s" s="1" r="I129">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="130">
       <c t="s" s="1" r="A130">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c s="1" r="B130">
         <v>117.0</v>
       </c>
       <c t="s" s="1" r="C130">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c t="s" s="2" r="D130">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c t="s" s="1" r="E130">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c t="s" s="2" r="F130">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c s="1" r="G130">
         <v>49590.0</v>
       </c>
       <c t="s" s="2" r="H130">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c t="str" r="I130">
-        <f ref="I130:I135" t="shared" si="5">iferror(iferror(REGEXEXTRACT(C130,"\((\w+)\)"),REGEXEXTRACT(E130,"\((\w+)\)")),"")</f>
+        <f ref="I130:I135" t="shared" si="6">iferror(iferror(REGEXEXTRACT(C130,"\((\w+)\)"),REGEXEXTRACT(E130,"\((\w+)\)")),"")</f>
         <v>OSTP</v>
       </c>
     </row>
     <row r="131">
       <c t="s" s="1" r="A131">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c s="1" r="B131">
         <v>57.0</v>
       </c>
       <c t="s" s="1" r="C131">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c t="s" s="2" r="D131">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c t="s" s="1" r="E131">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c t="s" s="2" r="F131">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c s="1" r="G131">
         <v>48081.0</v>
       </c>
       <c t="s" s="2" r="H131">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c t="str" r="I131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>NHTSA</v>
       </c>
     </row>
     <row r="132">
       <c t="s" s="1" r="A132">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c s="1" r="B132">
         <v>13.0</v>
       </c>
       <c t="s" s="1" r="C132">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c t="s" s="2" r="D132">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c t="s" s="1" r="E132">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c t="s" s="2" r="F132">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c s="1" r="G132">
         <v>52591.0</v>
       </c>
       <c t="s" s="2" r="H132">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c t="str" r="I132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CSB</v>
       </c>
     </row>
     <row r="133">
       <c t="s" s="1" r="A133">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c s="1" r="B133">
         <v>41.0</v>
       </c>
       <c t="s" s="1" r="C133">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c t="s" s="2" r="D133">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c t="s" s="1" r="E133">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c t="s" s="2" r="F133">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c s="1" r="G133">
         <v>49125.0</v>
       </c>
       <c t="s" s="2" r="H133">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c t="str" r="I133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>BLM</v>
       </c>
     </row>
     <row r="134">
       <c t="s" s="1" r="A134">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c s="1" r="B134">
         <v>30.0</v>
       </c>
       <c t="s" s="1" r="C134">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c t="s" s="2" r="D134">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c t="s" s="1" r="E134">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c t="s" s="2" r="F134">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c s="1" r="G134">
         <v>49530.0</v>
       </c>
       <c t="s" s="2" r="H134">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c t="str" r="I134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>NOAA</v>
       </c>
     </row>
     <row r="135">
       <c t="s" s="1" r="A135">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c s="1" r="B135">
         <v>140.0</v>
       </c>
       <c t="s" s="1" r="C135">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c t="s" s="2" r="D135">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c t="s" s="1" r="E135">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c t="s" s="2" r="F135">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c s="1" r="G135">
         <v>48029.0</v>
       </c>
       <c t="s" s="2" r="H135">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c t="str" r="I135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EBSA</v>
       </c>
     </row>
     <row r="136">
       <c t="s" s="3" r="A136">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c s="3" r="B136">
         <v>9.0</v>
       </c>
       <c t="s" s="3" r="C136">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c t="s" s="4" r="D136">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c t="s" s="3" r="E136">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c t="s" s="4" r="F136">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c s="3" r="G136">
         <v>91390.0</v>
       </c>
-      <c s="7" r="H136"/>
+      <c s="10" r="H136"/>
       <c t="s" s="3" r="I136">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="137">
       <c t="s" s="1" r="A137">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c s="1" r="B137">
         <v>12.0</v>
       </c>
       <c t="s" s="1" r="C137">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c t="s" s="2" r="D137">
-        <v>827</v>
-      </c>
-      <c t="s" s="8" r="E137">
         <v>828</v>
       </c>
+      <c t="s" s="11" r="E137">
+        <v>829</v>
+      </c>
       <c t="s" s="2" r="F137">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c s="1" r="G137">
         <v>49157.0</v>
       </c>
       <c t="str" r="I137">
-        <f ref="I137:I153" t="shared" si="6">iferror(iferror(REGEXEXTRACT(C137,"\((\w+)\)"),REGEXEXTRACT(E137,"\((\w+)\)")),"")</f>
+        <f ref="I137:I153" t="shared" si="7">iferror(iferror(REGEXEXTRACT(C137,"\((\w+)\)"),REGEXEXTRACT(E137,"\((\w+)\)")),"")</f>
         <v>CPPBSD</v>
       </c>
     </row>
     <row r="138">
       <c t="s" s="1" r="A138">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c s="1" r="B138">
         <v>14.0</v>
       </c>
       <c t="s" s="1" r="C138">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c t="s" s="2" r="D138">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c t="s" s="1" r="E138">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c t="s" s="2" r="F138">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c s="1" r="G138">
         <v>49191.0</v>
       </c>
       <c t="str" r="I138">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>CSOSA</v>
       </c>
     </row>
     <row r="139">
       <c t="s" s="1" r="A139">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c s="1" r="B139">
         <v>18.0</v>
       </c>
       <c t="s" s="1" r="C139">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c t="s" s="2" r="D139">
-        <v>837</v>
-      </c>
-      <c t="s" s="9" r="E139">
         <v>838</v>
       </c>
+      <c t="s" s="12" r="E139">
+        <v>839</v>
+      </c>
       <c t="s" s="2" r="F139">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c s="1" r="G139">
         <v>55927.0</v>
       </c>
       <c t="str" r="I139">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>CBP</v>
       </c>
     </row>
     <row r="140">
       <c t="s" s="1" r="A140">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c s="1" r="B140">
         <v>21.0</v>
       </c>
       <c t="s" s="1" r="C140">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c t="s" s="2" r="D140">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c t="s" s="1" r="E140">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c t="s" s="2" r="F140">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c s="1" r="G140">
         <v>49711.0</v>
       </c>
       <c t="str" r="I140">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ICE</v>
       </c>
     </row>
     <row r="141">
       <c t="s" s="1" r="A141">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c s="1" r="B141">
         <v>25.0</v>
       </c>
       <c t="s" s="1" r="C141">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c t="s" s="2" r="D141">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c t="s" s="1" r="E141">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c t="s" s="2" r="F141">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c s="1" r="G141">
         <v>48005.0</v>
       </c>
       <c t="str" r="I141">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="142">
       <c t="s" s="1" r="A142">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c s="1" r="B142">
         <v>33.0</v>
       </c>
       <c t="s" s="1" r="C142">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c t="s" s="2" r="D142">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c t="s" s="1" r="E142">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c t="s" s="2" r="F142">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c t="s" s="1" r="G142">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c t="s" s="1" r="H142">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c t="str" r="I142">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="143">
       <c t="s" s="1" r="A143">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c s="1" r="B143">
         <v>48.0</v>
       </c>
       <c t="s" s="1" r="C143">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c t="s" s="2" r="D143">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c t="s" s="1" r="E143">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c t="s" s="2" r="F143">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c t="str" r="I143">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="144">
       <c t="s" s="1" r="A144">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c s="1" r="B144">
         <v>61.0</v>
       </c>
       <c t="s" s="1" r="C144">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c t="s" s="2" r="D144">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c t="s" s="1" r="E144">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c t="s" s="2" r="F144">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c s="1" r="G144">
         <v>52603.0</v>
       </c>
       <c t="str" r="I144">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>EXIM</v>
       </c>
     </row>
     <row r="145">
       <c t="s" s="1" r="A145">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c s="1" r="B145">
         <v>74.0</v>
       </c>
       <c t="s" s="1" r="C145">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c t="s" s="2" r="D145">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c t="s" s="1" r="E145">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c t="s" s="2" r="F145">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c t="str" r="I145">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FOMC</v>
       </c>
     </row>
     <row r="146">
       <c t="s" s="1" r="A146">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c s="1" r="B146">
         <v>80.0</v>
       </c>
       <c t="s" s="1" r="C146">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c t="s" s="2" r="D146">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c t="s" s="1" r="E146">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c t="s" s="2" r="F146">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c t="str" r="I146">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ACL</v>
       </c>
     </row>
     <row r="147">
       <c t="s" s="1" r="A147">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c s="1" r="B147">
         <v>83.0</v>
       </c>
       <c t="s" s="1" r="C147">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c t="s" s="2" r="D147">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c t="s" s="1" r="E147">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c t="s" s="2" r="F147">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c s="1" r="G147">
         <v>49134.0</v>
       </c>
       <c t="str" r="I147">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>CMS</v>
       </c>
     </row>
     <row r="148">
       <c t="s" s="1" r="A148">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c s="1" r="B148">
         <v>88.0</v>
       </c>
       <c t="s" s="1" r="C148">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c t="s" s="2" r="D148">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c t="s" s="1" r="E148">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c t="s" s="2" r="F148">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c s="1" r="G148">
         <v>49687.0</v>
       </c>
       <c t="str" r="I148">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>SAMSHA</v>
       </c>
     </row>
     <row r="149">
       <c t="s" s="1" r="A149">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c s="1" r="B149">
         <v>97.0</v>
       </c>
       <c t="s" s="1" r="C149">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c t="s" s="2" r="D149">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c t="s" s="1" r="E149">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c t="s" s="2" r="F149">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c t="str" r="I149">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>JPL</v>
       </c>
     </row>
     <row r="150">
       <c t="s" s="1" r="A150">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c s="1" r="B150">
         <v>105.0</v>
       </c>
       <c t="s" s="1" r="C150">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c t="s" s="2" r="D150">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c t="s" s="1" r="E150">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c t="s" s="2" r="F150">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c s="1" r="G150">
         <v>49084.0</v>
       </c>
       <c t="str" r="I150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>AMTRAK</v>
       </c>
     </row>
     <row r="151">
       <c t="s" s="1" r="A151">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c s="1" r="B151">
         <v>112.0</v>
       </c>
       <c t="s" s="1" r="C151">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c t="s" s="2" r="D151">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c t="s" s="1" r="E151">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c t="s" s="2" r="F151">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c t="str" r="I151">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ONHIR</v>
       </c>
     </row>
     <row r="152">
       <c t="s" s="1" r="A152">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c s="1" r="B152">
         <v>121.0</v>
       </c>
       <c t="s" s="1" r="C152">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c t="s" s="2" r="D152">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c t="s" s="1" r="E152">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c t="s" s="2" r="F152">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c t="str" r="I152">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>RATB</v>
       </c>
     </row>
     <row r="153">
       <c t="s" s="1" r="A153">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c s="1" r="B153">
         <v>124.0</v>
       </c>
       <c t="s" s="1" r="C153">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c t="s" s="2" r="D153">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c t="s" s="1" r="E153">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c t="s" s="2" r="F153">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c t="str" r="I153">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>SIGAR</v>
       </c>
     </row>
     <row r="154">
       <c t="s" s="3" r="A154">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c s="3" r="B154">
         <v>129.0</v>
       </c>
       <c t="s" s="3" r="C154">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c t="s" s="3" r="D154">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c t="s" s="3" r="E154">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c t="s" s="4" r="F154">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c s="3" r="G154">
         <v>49034.0</v>
       </c>
-      <c s="7" r="H154"/>
+      <c s="10" r="H154"/>
       <c t="s" s="3" r="I154">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row r="155">
       <c t="s" s="1" r="A155">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c s="1" r="B155">
         <v>132.0</v>
       </c>
       <c t="s" s="1" r="C155">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c t="s" s="2" r="D155">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c t="s" s="1" r="E155">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c t="s" s="2" r="F155">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c s="1" r="G155">
         <v>48126.0</v>
       </c>
       <c t="str" r="I155">
-        <f ref="I155:I162" t="shared" si="7">iferror(iferror(REGEXEXTRACT(C155,"\((\w+)\)"),REGEXEXTRACT(E155,"\((\w+)\)")),"")</f>
+        <f ref="I155:I162" t="shared" si="8">iferror(iferror(REGEXEXTRACT(C155,"\((\w+)\)"),REGEXEXTRACT(E155,"\((\w+)\)")),"")</f>
         <v>OCC</v>
       </c>
     </row>
     <row r="156">
       <c t="s" s="1" r="A156">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c s="1" r="B156">
         <v>133.0</v>
       </c>
       <c t="s" s="1" r="C156">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c t="s" s="2" r="D156">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c t="s" s="1" r="E156">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c t="s" s="2" r="F156">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c t="str" r="I156">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>FINCEN</v>
       </c>
     </row>
     <row r="157">
       <c t="s" s="1" r="A157">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c s="1" r="B157">
         <v>141.0</v>
       </c>
       <c t="s" s="1" r="C157">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c t="s" s="2" r="D157">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c t="s" s="1" r="E157">
-        <v>931</v>
-      </c>
-      <c t="s" s="10" r="F157">
         <v>932</v>
+      </c>
+      <c t="s" s="13" r="F157">
+        <v>933</v>
       </c>
       <c s="1" r="G157">
         <v>52693.0</v>
       </c>
       <c t="str" r="I157">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DOLETA</v>
       </c>
     </row>
     <row r="158">
       <c t="s" s="1" r="A158">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c s="1" r="B158">
         <v>142.0</v>
       </c>
       <c t="s" s="1" r="C158">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c t="s" s="2" r="D158">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c t="s" s="1" r="E158">
-        <v>936</v>
-      </c>
-      <c t="s" s="10" r="F158">
         <v>937</v>
+      </c>
+      <c t="s" s="13" r="F158">
+        <v>938</v>
       </c>
       <c s="1" r="G158">
         <v>49462.0</v>
       </c>
       <c t="str" r="I158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>MSHA</v>
       </c>
     </row>
     <row r="159">
       <c t="s" s="1" r="A159">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c s="1" r="B159">
         <v>149.0</v>
       </c>
       <c t="s" s="1" r="C159">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c t="s" s="2" r="D159">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c t="s" s="1" r="E159">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c t="s" s="2" r="F159">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c t="str" r="I159">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>IBWC</v>
       </c>
     </row>
     <row r="160">
       <c t="s" s="1" r="A160">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c s="1" r="B160">
         <v>150.0</v>
       </c>
       <c t="s" s="1" r="C160">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c t="s" s="2" r="D160">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c t="s" s="1" r="E160">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c t="s" s="2" r="F160">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c s="1" r="G160">
         <v>49712.0</v>
       </c>
       <c t="str" r="I160">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>USITC</v>
       </c>
     </row>
     <row r="161">
       <c t="s" s="1" r="A161">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c s="1" r="B161">
         <v>153.0</v>
       </c>
       <c t="s" s="1" r="C161">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c t="s" s="2" r="D161">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c t="s" s="1" r="E161">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c t="s" s="2" r="F161">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c s="1" r="G161"/>
       <c t="str" r="I161">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="162">
       <c t="s" s="1" r="A162">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c s="1" r="B162">
         <v>154.0</v>
       </c>
       <c t="s" s="1" r="C162">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c t="s" s="2" r="D162">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c t="s" s="1" r="E162">
-        <v>956</v>
-      </c>
-      <c t="s" s="10" r="F162">
         <v>957</v>
+      </c>
+      <c t="s" s="13" r="F162">
+        <v>958</v>
       </c>
       <c s="1" r="G162">
         <v>49721.0</v>
       </c>
       <c t="str" r="I162">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>USTDA</v>
       </c>
     </row>
     <row r="163">
       <c t="s" s="3" r="A163">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c s="3" r="B163">
         <v>155.0</v>
       </c>
       <c t="s" s="3" r="C163">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c t="s" s="4" r="D163">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c t="s" s="3" r="E163">
-        <v>961</v>
-      </c>
-      <c t="s" s="11" r="F163">
         <v>962</v>
+      </c>
+      <c t="s" s="14" r="F163">
+        <v>963</v>
       </c>
       <c s="3" r="G163">
         <v>49724.0</v>
       </c>
-      <c s="7" r="H163"/>
+      <c s="10" r="H163"/>
       <c t="s" s="3" r="I163">
-        <v>963</v>
+        <v>964</v>
       </c>
     </row>
   </sheetData>
@@ -8501,46 +8522,46 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c t="s" s="1" r="C1">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c t="s" s="1" r="D1">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c t="s" s="1" r="E1">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c t="s" s="1" r="F1">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c t="s" s="1" r="G1">
-        <v>970</v>
-      </c>
-      <c s="12" r="H1"/>
+        <v>971</v>
+      </c>
+      <c s="15" r="H1"/>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c t="s" s="2" r="D2">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c t="s" s="1" r="F2">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c t="str" r="G2">
         <f ref="G2:G12" t="shared" si="1">iferror(iferror(REGEXEXTRACT(A2,"\((\w+)\)"),REGEXEXTRACT(C2,"\((\w+)\)")),"")</f>
@@ -8549,16 +8570,16 @@
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c t="s" s="2" r="B3">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c t="s" s="2" r="D3">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c t="str" r="G3">
         <f t="shared" si="1"/>
@@ -8567,16 +8588,16 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c t="s" s="2" r="B4">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c t="s" s="2" r="D4">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c t="str" r="G4">
         <f t="shared" si="1"/>
@@ -8585,16 +8606,16 @@
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c t="s" s="2" r="B5">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c t="s" s="2" r="D5">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c t="str" r="G5">
         <f t="shared" si="1"/>
@@ -8603,16 +8624,16 @@
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c t="s" s="2" r="B6">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c t="s" s="2" r="D6">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c t="str" r="G6">
         <f t="shared" si="1"/>
@@ -8621,16 +8642,16 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c t="s" s="2" r="B7">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c t="s" s="2" r="D7">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c t="str" r="G7">
         <f t="shared" si="1"/>
@@ -8639,16 +8660,16 @@
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c t="s" s="2" r="B8">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c t="s" s="2" r="D8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c t="str" r="G8">
         <f t="shared" si="1"/>
@@ -8657,16 +8678,16 @@
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c t="s" s="2" r="B9">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c t="s" s="2" r="D9">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c t="str" r="G9">
         <f t="shared" si="1"/>
@@ -8675,16 +8696,16 @@
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c t="s" s="2" r="B10">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c t="s" s="2" r="D10">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c t="str" r="G10">
         <f t="shared" si="1"/>
@@ -8693,16 +8714,16 @@
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c t="s" s="2" r="B11">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c t="s" s="2" r="D11">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c t="str" r="G11">
         <f t="shared" si="1"/>
@@ -8711,16 +8732,16 @@
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c t="s" s="2" r="B12">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c t="s" s="2" r="D12">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c s="1" r="E12"/>
       <c t="str" r="G12">

</xml_diff>